<commit_message>
L4 - Added Spreadsheet for hall voltage data.
</commit_message>
<xml_diff>
--- a/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
+++ b/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2DAD47-9BAA-4831-A3E9-66D1F222AFC6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7394AC20-7982-4BF5-9B5F-075BCFF2E3DA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration of Electromagnet" sheetId="1" r:id="rId1"/>
+    <sheet name="Hall Voltage Measurements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -19,20 +20,94 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{D40F77C3-51C3-4760-9775-62DC113AEDF9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Read of gauss probe</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A01E4D02-61CF-44F3-AB95-3E61E3235764}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From equaiton 13 in lab manual
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">Current (A) </t>
   </si>
   <si>
     <t>Magnetic Field (T)</t>
   </si>
+  <si>
+    <t>Electromagnet Current 1 (A)</t>
+  </si>
+  <si>
+    <t>Electromagnet Current 2 (A)</t>
+  </si>
+  <si>
+    <t>Hall Voltage 2 (V)</t>
+  </si>
+  <si>
+    <t>Hall Voltage 1 (V)</t>
+  </si>
+  <si>
+    <t>Offset Hall Voltage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,6 +122,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -77,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +745,561 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Electromagnetic Field vs Hall Voltage</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hall Voltage Measurements'!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hall Voltage Measurements'!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F2A1-4AC3-AA79-B152765A106F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="461534912"/>
+        <c:axId val="461536224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="461534912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Electromagnetic Field (T)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461536224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="461536224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hall Voltage (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="461534912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1212,6 +1855,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1233,6 +2392,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E9451F-6E22-46CC-8B08-3C9BD55FA770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94C6EF6D-522E-4F46-BECC-46A9730E595B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1518,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -1684,4 +2884,282 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B218D3DE-8ED2-47E4-8CF9-EB74F10691A2}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>0.5*(B2-D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.25</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="F3">
+        <f>0.5*(A3-C3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>0.25 + A3</f>
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <f>0.25 + C3</f>
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <f>0.5*(A4-C4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>0.25 + A4</f>
+        <v>0.75</v>
+      </c>
+      <c r="C5">
+        <f>0.25 + C4</f>
+        <v>0.75</v>
+      </c>
+      <c r="F5">
+        <f>0.5*(A5-C5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>0.25 + A5</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>0.25 + C5</f>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>0.5*(A6-C6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>0.25 + A6</f>
+        <v>1.25</v>
+      </c>
+      <c r="C7">
+        <f>0.25 + C6</f>
+        <v>1.25</v>
+      </c>
+      <c r="F7">
+        <f>0.5*(A7-C7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>0.25 + A7</f>
+        <v>1.5</v>
+      </c>
+      <c r="C8">
+        <f>0.25 + C7</f>
+        <v>1.5</v>
+      </c>
+      <c r="F8">
+        <f>0.5*(A8-C8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>0.25 + A8</f>
+        <v>1.75</v>
+      </c>
+      <c r="C9">
+        <f>0.25 + C8</f>
+        <v>1.75</v>
+      </c>
+      <c r="F9">
+        <f>0.5*(A9-C9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>0.25 + A9</f>
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f>0.25 + C9</f>
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f>0.5*(A10-C10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>0.25 + A10</f>
+        <v>2.25</v>
+      </c>
+      <c r="C11">
+        <f>0.25 + C10</f>
+        <v>2.25</v>
+      </c>
+      <c r="F11">
+        <f>0.5*(A11-C11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>0.25 + A11</f>
+        <v>2.5</v>
+      </c>
+      <c r="C12">
+        <f>0.25 + C11</f>
+        <v>2.5</v>
+      </c>
+      <c r="F12">
+        <f>0.5*(A12-C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>0.25 + A12</f>
+        <v>2.75</v>
+      </c>
+      <c r="C13">
+        <f>0.25 + C12</f>
+        <v>2.75</v>
+      </c>
+      <c r="F13">
+        <f>0.5*(A13-C13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>0.25 + A13</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>0.25 + C13</f>
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f>0.5*(A14-C14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>0.25 + A14</f>
+        <v>3.25</v>
+      </c>
+      <c r="C15">
+        <f>0.25 + C14</f>
+        <v>3.25</v>
+      </c>
+      <c r="F15">
+        <f>0.5*(A15-C15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>0.25 + A15</f>
+        <v>3.5</v>
+      </c>
+      <c r="C16">
+        <f>0.25 + C15</f>
+        <v>3.5</v>
+      </c>
+      <c r="F16">
+        <f>0.5*(A16-C16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>0.25 + A16</f>
+        <v>3.75</v>
+      </c>
+      <c r="C17">
+        <f>0.25 + C16</f>
+        <v>3.75</v>
+      </c>
+      <c r="F17">
+        <f>0.5*(A17-C17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>0.25 + A17</f>
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f>0.25 + C17</f>
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f>0.5*(A18-C18)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed: abstract, introduction, procedures and results.
Need to do discussion and conclusion.
</commit_message>
<xml_diff>
--- a/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
+++ b/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6E37AC-B713-4B49-9DF7-44881C863DF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAF2033-3104-422E-AA94-319F05E19F2E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -848,7 +848,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Electromagnetic Field vs Hall Voltage</a:t>
+              <a:t>Electromagnetic Field vs Offset Voltage</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1412,7 +1412,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Magnetic Field vs Voltage</a:t>
+              <a:t>Magnetic Field vs Offset Voltage</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3660,8 +3660,8 @@
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
@@ -3696,15 +3696,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1033462</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4731,7 +4731,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed lab 4 - hall effect
</commit_message>
<xml_diff>
--- a/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
+++ b/Labs/Lab 4 - Investigation of the Hall Effect in Semiconductors/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAF2033-3104-422E-AA94-319F05E19F2E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B112DAF0-49A6-4AC6-98F5-2792380ADFB3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration of Electromagnet 2" sheetId="4" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t xml:space="preserve">Current (A) </t>
   </si>
@@ -164,6 +164,27 @@
   </si>
   <si>
     <t>Hall Voltage 2 (mV)</t>
+  </si>
+  <si>
+    <t>+5%</t>
+  </si>
+  <si>
+    <t>+5 to -5 grad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5 to +5 grad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original </t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Difference (%)</t>
+  </si>
+  <si>
+    <t>Scaled</t>
   </si>
 </sst>
 </file>
@@ -220,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +259,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,6 +1106,216 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>-5 to +5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.61391318659424998"/>
+                  <c:y val="0.38342235410484671"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Voltage Measurements 3361 Ge'!$E$2,'Voltage Measurements 3361 Ge'!$E$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Voltage Measurements 3361 Ge'!$H$2,'Voltage Measurements 3361 Ge'!$I$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-1.1550000000000017E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.65597499999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-24B1-432A-92FC-8AECF9202EF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>-5 to +5 </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.21313582377545273"/>
+                  <c:y val="0.50203832687232519"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Voltage Measurements 3361 Ge'!$E$2,'Voltage Measurements 3361 Ge'!$E$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Voltage Measurements 3361 Ge'!$I$2,'Voltage Measurements 3361 Ge'!$H$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-1.0450000000000013E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.72502500000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-24B1-432A-92FC-8AECF9202EF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3654,16 +3890,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4246,19 +4482,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B218D3DE-8ED2-47E4-8CF9-EB74F10691A2}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -4277,8 +4517,14 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="8">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>0</f>
         <v>0</v>
@@ -4303,8 +4549,16 @@
         <f>F2*0.01</f>
         <v>-1.1000000000000015E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>F2*1.05</f>
+        <v>-1.1550000000000017E-2</v>
+      </c>
+      <c r="I2">
+        <f>F2*0.95</f>
+        <v>-1.0450000000000013E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.25</v>
       </c>
@@ -4328,7 +4582,7 @@
         <v>-5.8999999999999992E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A18" si="1">0.25 + A3</f>
         <v>0.5</v>
@@ -4354,7 +4608,7 @@
         <v>-1.0649999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>0.75</v>
@@ -4380,7 +4634,7 @@
         <v>-1.5499999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4406,7 +4660,7 @@
         <v>-2.0300000000000006E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>1.25</v>
@@ -4432,7 +4686,7 @@
         <v>-2.5049999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>1.5</v>
@@ -4458,7 +4712,7 @@
         <v>-2.98E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>1.75</v>
@@ -4484,7 +4738,7 @@
         <v>-3.4399999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -4510,7 +4764,7 @@
         <v>-3.8799999999999998E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>2.25</v>
@@ -4536,7 +4790,7 @@
         <v>-4.3350000000000012E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>2.5</v>
@@ -4562,7 +4816,7 @@
         <v>-4.7450000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>2.75</v>
@@ -4588,7 +4842,7 @@
         <v>-5.1249999999999993E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -4614,7 +4868,7 @@
         <v>-5.5050000000000003E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>3.25</v>
@@ -4640,7 +4894,7 @@
         <v>-5.8899999999999994E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>3.5</v>
@@ -4666,7 +4920,7 @@
         <v>-6.2300000000000012E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>3.75</v>
@@ -4692,7 +4946,7 @@
         <v>-6.5750000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4716,6 +4970,81 @@
       <c r="G18">
         <f t="shared" si="0"/>
         <v>-6.9050000000000005E-3</v>
+      </c>
+      <c r="H18">
+        <f>F18*1.05</f>
+        <v>-0.72502500000000003</v>
+      </c>
+      <c r="I18">
+        <f>F18*0.95</f>
+        <v>-0.65597499999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>0.2064</v>
+      </c>
+      <c r="I20">
+        <f>1-H20/0.2064</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>0.2064-0.1956</f>
+        <v>1.0800000000000004E-2</v>
+      </c>
+      <c r="K20">
+        <f>J20*100000</f>
+        <v>1080.0000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>0.1956</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I22" si="3">1-H21/0.2064</f>
+        <v>5.2325581395348819E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>-5.0872093023255793E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f>0.2064*1.052</f>
+        <v>0.21713280000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f>3.33*0.05</f>
+        <v>0.16650000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4730,7 +5059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4687F6FE-006E-406B-A4E2-9E9461A00185}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>

</xml_diff>